<commit_message>
fix: added atribute deleted and added lombok's dependency
</commit_message>
<xml_diff>
--- a/theory/Dabase Model R.xlsx
+++ b/theory/Dabase Model R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56949\Desktop\MyHomeworks\Acceso por carpetas\De Carrera\9 semestre\arq de sistemas\segunda vez\talleres\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAB484D-D4B0-40AE-BC73-C5BDB2727974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EAAE38-9758-4424-941A-1DD0CC7EE588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>EntityCard</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>power (from potential)</t>
-  </si>
-  <si>
     <t>physical power</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>TypeId</t>
+  </si>
+  <si>
+    <t>deleted</t>
   </si>
 </sst>
 </file>
@@ -436,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J16"/>
+  <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -463,27 +463,30 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -497,21 +500,21 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
@@ -522,12 +525,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>